<commit_message>
update canonical url (#81) 917ea08017fd841cdd24511ee1ec181b6f2e9fef
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-fr-additional-when-codes.xlsx
+++ b/main/ig/CodeSystem-fr-additional-when-codes.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://hl7.fr/fhir/fr/medication/CodeSystem/fr-additional-when-codes</t>
+    <t>https://hl7.fr/ig/fhir/medication/CodeSystem/fr-additional-when-codes</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-05T07:40:26+00:00</t>
+    <t>2025-05-05T08:11:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>